<commit_message>
Added mySQL to upload service
</commit_message>
<xml_diff>
--- a/stock_prices.xlsx
+++ b/stock_prices.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Educational\SocGen Training material\Final_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Educational\SocGenTraininMaterial\Final_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACD2FBCD-1691-495D-BDE6-F3A559778EB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C55CB22E-8F88-4316-8E93-FF388B8992D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2505" yWindow="4080" windowWidth="15915" windowHeight="9150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="15915" windowHeight="9150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
   <si>
     <t>Company Code</t>
   </si>
@@ -40,9 +40,6 @@
   </si>
   <si>
     <t>Time</t>
-  </si>
-  <si>
-    <t>500112 </t>
   </si>
   <si>
     <t>BSE</t>
@@ -394,7 +391,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -417,11 +414,11 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
+      <c r="A2">
+        <v>500112</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2">
         <v>356.23</v>
@@ -430,15 +427,15 @@
         <v>43624</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
+      <c r="A3">
+        <v>500112</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3">
         <v>361.31</v>
@@ -447,15 +444,15 @@
         <v>43624</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
+      <c r="A4">
+        <v>500112</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4">
         <v>358.12</v>
@@ -464,15 +461,15 @@
         <v>43624</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
+      <c r="A5">
+        <v>500112</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5">
         <v>357.09</v>
@@ -481,15 +478,15 @@
         <v>43624</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
+      <c r="A6">
+        <v>500112</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6">
         <v>353.62</v>
@@ -498,15 +495,15 @@
         <v>43624</v>
       </c>
       <c r="E6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>5</v>
+      <c r="A7">
+        <v>500112</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7">
         <v>349.56</v>
@@ -515,15 +512,15 @@
         <v>43624</v>
       </c>
       <c r="E7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>5</v>
+      <c r="A8">
+        <v>500112</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8">
         <v>351.43</v>
@@ -532,15 +529,15 @@
         <v>43624</v>
       </c>
       <c r="E8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>5</v>
+      <c r="A9">
+        <v>500112</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9">
         <v>350.12</v>
@@ -549,15 +546,15 @@
         <v>43624</v>
       </c>
       <c r="E9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>5</v>
+      <c r="A10">
+        <v>500112</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C10">
         <v>348.91</v>
@@ -566,7 +563,7 @@
         <v>43624</v>
       </c>
       <c r="E10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed front end admin company functionality:=
</commit_message>
<xml_diff>
--- a/stock_prices.xlsx
+++ b/stock_prices.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Educational\SocGenTraininMaterial\Final_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C55CB22E-8F88-4316-8E93-FF388B8992D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAC47464-3C6B-400B-A565-E156C5B5350C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1170" yWindow="1170" windowWidth="15915" windowHeight="9150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,9 +36,6 @@
     <t>Price Per Share(in Rs)</t>
   </si>
   <si>
-    <t xml:space="preserve">Date </t>
-  </si>
-  <si>
     <t>Time</t>
   </si>
   <si>
@@ -70,6 +67,9 @@
   </si>
   <si>
     <t xml:space="preserve">  11:10:00</t>
+  </si>
+  <si>
+    <t>date</t>
   </si>
 </sst>
 </file>
@@ -391,7 +391,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -406,11 +406,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -418,16 +418,16 @@
         <v>500112</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2">
         <v>356.23</v>
       </c>
       <c r="D2" s="1">
-        <v>43624</v>
+        <v>36714</v>
       </c>
       <c r="E2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -435,16 +435,16 @@
         <v>500112</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3">
         <v>361.31</v>
       </c>
       <c r="D3" s="1">
-        <v>43624</v>
+        <v>36714</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -452,16 +452,16 @@
         <v>500112</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4">
         <v>358.12</v>
       </c>
       <c r="D4" s="1">
-        <v>43624</v>
+        <v>36714</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -469,16 +469,16 @@
         <v>500112</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5">
         <v>357.09</v>
       </c>
       <c r="D5" s="1">
-        <v>43624</v>
+        <v>36714</v>
       </c>
       <c r="E5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -486,16 +486,16 @@
         <v>500112</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6">
         <v>353.62</v>
       </c>
       <c r="D6" s="1">
-        <v>43624</v>
+        <v>36714</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -503,16 +503,16 @@
         <v>500112</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7">
         <v>349.56</v>
       </c>
       <c r="D7" s="1">
-        <v>43624</v>
+        <v>36714</v>
       </c>
       <c r="E7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -520,16 +520,16 @@
         <v>500112</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8">
         <v>351.43</v>
       </c>
       <c r="D8" s="1">
-        <v>43624</v>
+        <v>36714</v>
       </c>
       <c r="E8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -537,16 +537,16 @@
         <v>500112</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C9">
         <v>350.12</v>
       </c>
       <c r="D9" s="1">
-        <v>43624</v>
+        <v>36714</v>
       </c>
       <c r="E9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -554,16 +554,16 @@
         <v>500112</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C10">
         <v>348.91</v>
       </c>
       <c r="D10" s="1">
-        <v>43624</v>
+        <v>36714</v>
       </c>
       <c r="E10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>